<commit_message>
update template files used when create new file
fix "Vincent Lee is author of all Word files created in Seahub"
</commit_message>
<xml_diff>
--- a/media/office-template/empty.xlsx
+++ b/media/office-template/empty.xlsx
@@ -1,27 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17626"/>
-  <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2ACDA410-FDA2-4D24-815A-ED1A93F7A727}" xr6:coauthVersionLast="12" xr6:coauthVersionMax="12" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102B4B57-6F0B-4FA0-9ADA-141DB9E8C2D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171026"/>
+  <calcPr calcId="162913"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -52,7 +64,7 @@
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -75,44 +87,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="085296"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="993366"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -142,12 +154,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -186,166 +198,142 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
@@ -353,10 +341,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update pptx/xlsx office template
</commit_message>
<xml_diff>
--- a/media/office-template/empty.xlsx
+++ b/media/office-template/empty.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102B4B57-6F0B-4FA0-9ADA-141DB9E8C2D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457521CB-5AA5-4971-BF0F-36763508E5DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1368" yWindow="372" windowWidth="19488" windowHeight="8964" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150000" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -21,17 +24,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="DengXian"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -64,7 +67,7 @@
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -122,9 +125,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -157,9 +160,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -343,7 +346,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.6"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update pptx/xlsx office template (#4340)
</commit_message>
<xml_diff>
--- a/media/office-template/empty.xlsx
+++ b/media/office-template/empty.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102B4B57-6F0B-4FA0-9ADA-141DB9E8C2D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457521CB-5AA5-4971-BF0F-36763508E5DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1368" yWindow="372" windowWidth="19488" windowHeight="8964" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150000" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -21,17 +24,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="DengXian"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -64,7 +67,7 @@
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -122,9 +125,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -157,9 +160,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -343,7 +346,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.6"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>